<commit_message>
Edit before finish branch
</commit_message>
<xml_diff>
--- a/docs/Report.xlsx
+++ b/docs/Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fzopr\Documents\Code\Collabarator\rov-item-recommender\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82A70B7-123A-4497-A686-E8778F22F31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3475FA0-B592-4974-ACDD-9DFBEEF3602D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>ลำดับ</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>แก้ไข Select Farm Item ไม่ขึ่น</t>
+  </si>
+  <si>
+    <t>สถานะ</t>
+  </si>
+  <si>
+    <t>ยังไม่ได้แก้ไข</t>
+  </si>
+  <si>
+    <t>แก้ไขแล้ว</t>
+  </si>
+  <si>
+    <t>แก้ไขให้แสดงเมื่อเลือก Farm Lane ใน Select Lane</t>
+  </si>
+  <si>
+    <t>แก้ไขให้แสดงเมื่อเลือก Support Lane ใน Select Lane</t>
   </si>
 </sst>
 </file>
@@ -75,12 +90,24 @@
       <name val="Sukhumvit Set"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -95,9 +122,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -106,6 +139,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -380,21 +418,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="27.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="27.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.54296875" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="66.6328125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="66.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -404,8 +443,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -415,8 +457,11 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -426,8 +471,11 @@
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -437,8 +485,11 @@
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -447,6 +498,92 @@
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit Select Class, Select Lane, Support Item, Farm Item
</commit_message>
<xml_diff>
--- a/docs/Report.xlsx
+++ b/docs/Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fzopr\Documents\Code\Collabarator\rov-item-recommender\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\RoV-Item-Recommender-System\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4150F85E-B20E-4693-B10C-08DFBBBD876E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB76C87-8A39-4585-B166-5298CB97232A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2370" yWindow="2865" windowWidth="21630" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,29 +137,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -445,311 +442,191 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="27.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="20.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="66.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.08984375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="66.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
+    <row r="2" spans="1:4" ht="33.6" customHeight="1">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>